<commit_message>
feat: add feature to obtain the info from an excel file
</commit_message>
<xml_diff>
--- a/Registro_Tiempos_TW.xlsx
+++ b/Registro_Tiempos_TW.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alfredo/Documents/Desarrollo/Testing/playwright/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\luis.parra\Documents\VSCode\Python\record_times_tw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26DA8E3-6C73-DE46-A54D-70DABB36BA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEC6B72-2FDF-4169-8239-999E349DB3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{712FD5F4-F01D-304E-AC2D-B90A5CFF0874}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="20700" windowHeight="8700" xr2:uid="{712FD5F4-F01D-304E-AC2D-B90A5CFF0874}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,6 +33,41 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Hora Inicio</t>
+  </si>
+  <si>
+    <t>Hora Fin</t>
+  </si>
+  <si>
+    <t>Tiempo Dedicado</t>
+  </si>
+  <si>
+    <t>Tarea TW</t>
+  </si>
+  <si>
+    <t>Desayunar</t>
+  </si>
+  <si>
+    <t>tw/breakfast</t>
+  </si>
+  <si>
+    <t>Almorzar</t>
+  </si>
+  <si>
+    <t>tw/launch</t>
+  </si>
+  <si>
+    <t>Descripción Tarea</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,9 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,16 +423,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AF72DF-7CD3-E649-862E-1CF7D170BAB2}">
-  <dimension ref="B2"/>
+  <dimension ref="B1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>20231209</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F2" s="3">
+        <f>E2-D2</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>20231209</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F3" s="3">
+        <f>E3-D3</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add validations to errors with try-catch
</commit_message>
<xml_diff>
--- a/Registro_Tiempos_TW.xlsx
+++ b/Registro_Tiempos_TW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\luis.parra\Documents\VSCode\Python\record_times_tw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEC6B72-2FDF-4169-8239-999E349DB3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98F04E5-02C6-4E9B-B721-777BC7F334EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="20700" windowHeight="8700" xr2:uid="{712FD5F4-F01D-304E-AC2D-B90A5CFF0874}"/>
+    <workbookView xWindow="21270" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{712FD5F4-F01D-304E-AC2D-B90A5CFF0874}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Fecha</t>
   </si>
@@ -53,19 +53,13 @@
     <t>Tarea TW</t>
   </si>
   <si>
-    <t>Desayunar</t>
-  </si>
-  <si>
-    <t>tw/breakfast</t>
-  </si>
-  <si>
-    <t>Almorzar</t>
-  </si>
-  <si>
-    <t>tw/launch</t>
-  </si>
-  <si>
     <t>Descripción Tarea</t>
+  </si>
+  <si>
+    <t>Vacaciones</t>
+  </si>
+  <si>
+    <t>https://grupocadena.teamwork.com/app/tasks/33794025</t>
   </si>
 </sst>
 </file>
@@ -75,8 +69,30 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,16 +117,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,85 +462,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AF72DF-7CD3-E649-862E-1CF7D170BAB2}">
-  <dimension ref="B1:G3"/>
+  <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="11" style="1"/>
+    <col min="2" max="2" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>20231209</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45279</v>
+      </c>
+      <c r="D2" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E2" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F2" s="5">
         <f>E2-D2</f>
-        <v>4.1666666666666685E-2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45280</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F3" s="5">
+        <f>E3-D3</f>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>20231209</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F3" s="3">
-        <f>E3-D3</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7">
+        <v>45281</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F5" si="0">E4-D4</f>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>45282</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="8"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{D136061D-FCC7-4772-A19D-FCBF6AD1A942}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{D97AF88F-EA86-441C-A883-A44387BA714C}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{1135DFFC-5200-48F9-8D5A-58E038ECAFB0}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{03FC7952-B758-45B6-B5DA-E398D9A24945}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>